<commit_message>
Uploading participants data and survey analysis
</commit_message>
<xml_diff>
--- a/survey_data.xlsx
+++ b/survey_data.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conso\OneDrive\Documents\GitHub\robot-barriers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84299CBC-F333-4863-A600-30C1C577CA83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C053A796-C473-4B75-ACCF-C55F395332C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Former Experience" sheetId="1" r:id="rId1"/>
+    <sheet name="Former Programming Experience" sheetId="1" r:id="rId1"/>
     <sheet name="Former Content Experience" sheetId="2" r:id="rId2"/>
     <sheet name="Desktop Feedback" sheetId="4" r:id="rId3"/>
     <sheet name="Programming Feedback" sheetId="5" r:id="rId4"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="183">
   <si>
     <t>How many years of experience do you have in computer programming?</t>
   </si>
@@ -570,6 +570,33 @@
   </si>
   <si>
     <t>%</t>
+  </si>
+  <si>
+    <t>Computer Programming Experience (Years)</t>
+  </si>
+  <si>
+    <t>Block-Based Programming Experience (Years)</t>
+  </si>
+  <si>
+    <t>Robot Programming Experience (Years)</t>
+  </si>
+  <si>
+    <t>Level of Experience in Robotics</t>
+  </si>
+  <si>
+    <t>Experienced</t>
+  </si>
+  <si>
+    <t>Highly experienced</t>
+  </si>
+  <si>
+    <t>Year in College</t>
+  </si>
+  <si>
+    <t>Freshman</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
 </sst>
 </file>
@@ -577,7 +604,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="m/d/yyyy\ h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -693,7 +720,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -746,7 +773,7 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -767,6 +794,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1053,19 +1081,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="10.89453125" style="11" customWidth="1"/>
     <col min="2" max="6" width="40.578125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="40.26171875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="56.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="56.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="9" t="s">
         <v>81</v>
       </c>
@@ -1084,8 +1113,15 @@
       <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H1" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="I1" s="22">
+        <f>COUNTA(A2:A50)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="10" t="s">
         <v>57</v>
       </c>
@@ -1105,7 +1141,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="10" t="s">
         <v>58</v>
       </c>
@@ -1124,8 +1160,17 @@
       <c r="F3" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H3" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="10" t="s">
         <v>59</v>
       </c>
@@ -1144,8 +1189,19 @@
       <c r="F4" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <f>COUNTIF($B$2:$B$50, H4)</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="25">
+        <f>I4/$I$1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="10" t="s">
         <v>60</v>
       </c>
@@ -1164,8 +1220,19 @@
       <c r="F5" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H5" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ref="I5:I8" si="0">COUNTIF($B$2:$B$50, H5)</f>
+        <v>1</v>
+      </c>
+      <c r="J5" s="25">
+        <f t="shared" ref="J5:J8" si="1">I5/$I$1</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="10" t="s">
         <v>61</v>
       </c>
@@ -1184,8 +1251,19 @@
       <c r="F6" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H6" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="J6" s="25">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="10" t="s">
         <v>62</v>
       </c>
@@ -1204,8 +1282,19 @@
       <c r="F7" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H7" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="J7" s="25">
+        <f t="shared" si="1"/>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="10" t="s">
         <v>63</v>
       </c>
@@ -1224,8 +1313,19 @@
       <c r="F8" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H8" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J8" s="25">
+        <f t="shared" si="1"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="10" t="s">
         <v>64</v>
       </c>
@@ -1245,7 +1345,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="10" t="s">
         <v>65</v>
       </c>
@@ -1264,8 +1364,17 @@
       <c r="F10" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H10" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="10" t="s">
         <v>66</v>
       </c>
@@ -1284,8 +1393,19 @@
       <c r="F11" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I11">
+        <f>COUNTIF($C$2:$C$50, H11)</f>
+        <v>13</v>
+      </c>
+      <c r="J11" s="25">
+        <f>I11/$I$1</f>
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="10" t="s">
         <v>67</v>
       </c>
@@ -1304,8 +1424,19 @@
       <c r="F12" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H12" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="I12">
+        <f t="shared" ref="I12:I15" si="2">COUNTIF($C$2:$C$50, H12)</f>
+        <v>6</v>
+      </c>
+      <c r="J12" s="25">
+        <f t="shared" ref="J12:J15" si="3">I12/$I$1</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="10" t="s">
         <v>68</v>
       </c>
@@ -1324,8 +1455,19 @@
       <c r="F13" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H13" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="J13" s="25">
+        <f t="shared" si="3"/>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="10" t="s">
         <v>69</v>
       </c>
@@ -1344,8 +1486,19 @@
       <c r="F14" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H14" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="10" t="s">
         <v>70</v>
       </c>
@@ -1364,8 +1517,19 @@
       <c r="F15" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H15" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J15" s="25">
+        <f t="shared" si="3"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="10" t="s">
         <v>71</v>
       </c>
@@ -1385,7 +1549,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="10" t="s">
         <v>72</v>
       </c>
@@ -1404,8 +1568,17 @@
       <c r="F17" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H17" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="10" t="s">
         <v>73</v>
       </c>
@@ -1424,8 +1597,19 @@
       <c r="F18" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I18">
+        <f>COUNTIF($D$2:$D$50,H18)</f>
+        <v>20</v>
+      </c>
+      <c r="J18" s="25">
+        <f>I18/$I$1</f>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="10" t="s">
         <v>74</v>
       </c>
@@ -1444,8 +1628,19 @@
       <c r="F19" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H19" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="I19">
+        <f t="shared" ref="I19:I22" si="4">COUNTIF($D$2:$D$50,H19)</f>
+        <v>4</v>
+      </c>
+      <c r="J19" s="25">
+        <f t="shared" ref="J19:J22" si="5">I19/$I$1</f>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="10" t="s">
         <v>75</v>
       </c>
@@ -1464,8 +1659,19 @@
       <c r="F20" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H20" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J20" s="25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="10" t="s">
         <v>76</v>
       </c>
@@ -1484,8 +1690,19 @@
       <c r="F21" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H21" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J21" s="25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="10" t="s">
         <v>77</v>
       </c>
@@ -1504,8 +1721,19 @@
       <c r="F22" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H22" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J22" s="25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="10" t="s">
         <v>78</v>
       </c>
@@ -1525,7 +1753,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="10" t="s">
         <v>79</v>
       </c>
@@ -1544,8 +1772,17 @@
       <c r="F24" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H24" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="10" t="s">
         <v>80</v>
       </c>
@@ -1563,6 +1800,144 @@
       </c>
       <c r="F25" s="2" t="s">
         <v>3</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="I25">
+        <f>COUNTIF($E$2:$E$50,H25)</f>
+        <v>14</v>
+      </c>
+      <c r="J25" s="25">
+        <f>I25/$I$1</f>
+        <v>0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="H26" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I26">
+        <f t="shared" ref="I26:I29" si="6">COUNTIF($E$2:$E$50,H26)</f>
+        <v>8</v>
+      </c>
+      <c r="J26" s="25">
+        <f t="shared" ref="J26:J29" si="7">I26/$I$1</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="H27" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="J27" s="25">
+        <f t="shared" si="7"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="H28" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J28" s="25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="H29" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J29" s="25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="H31" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="H32" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="I32">
+        <f>COUNTIF($F$2:$F$50, H32)</f>
+        <v>0</v>
+      </c>
+      <c r="J32" s="25">
+        <f>I32/$I$1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="8:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="H33" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="I33">
+        <f t="shared" ref="I33:I36" si="8">COUNTIF($F$2:$F$50, H33)</f>
+        <v>1</v>
+      </c>
+      <c r="J33" s="25">
+        <f t="shared" ref="J33:J36" si="9">I33/$I$1</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="8:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="H34" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="J34" s="25">
+        <f t="shared" si="9"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="35" spans="8:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="H35" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="8"/>
+        <v>16</v>
+      </c>
+      <c r="J35" s="25">
+        <f t="shared" si="9"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="36" spans="8:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="H36" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="I36">
+        <v>1</v>
+      </c>
+      <c r="J36" s="25">
+        <f t="shared" si="9"/>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1574,8 +1949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C062337-35C7-4B37-8E97-B8F2FA166929}">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="L1" sqref="K1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2288,20 +2663,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5554D22B-F073-46F9-B62C-DC5D270AF810}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="10.89453125" style="13" customWidth="1"/>
-    <col min="2" max="9" width="40.578125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="40.578125" style="1" customWidth="1"/>
+    <col min="2" max="8" width="40.578125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="40.578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="48.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" ht="48.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="9" t="s">
         <v>81</v>
       </c>
@@ -2309,37 +2684,37 @@
         <v>86</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="J1" s="15" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="12" t="s">
         <v>57</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>98</v>
       </c>
+      <c r="C2" s="5" t="s">
+        <v>98</v>
+      </c>
       <c r="D2" s="5" t="s">
         <v>98</v>
       </c>
@@ -2355,11 +2730,8 @@
       <c r="H2" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="12" t="s">
         <v>58</v>
       </c>
@@ -2367,7 +2739,7 @@
         <v>99</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>101</v>
@@ -2384,11 +2756,8 @@
       <c r="H3" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="25.8" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="12" t="s">
         <v>59</v>
       </c>
@@ -2396,28 +2765,25 @@
         <v>99</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>97</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="25.8" x14ac:dyDescent="0.55000000000000004">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="25.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="12" t="s">
         <v>60</v>
       </c>
@@ -2425,13 +2791,13 @@
         <v>95</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>97</v>
@@ -2440,16 +2806,13 @@
         <v>97</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="I5" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="I5" s="6" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="12" t="s">
         <v>61</v>
       </c>
@@ -2457,7 +2820,7 @@
         <v>99</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>97</v>
@@ -2466,19 +2829,16 @@
         <v>97</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="51.6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="12" t="s">
         <v>62</v>
       </c>
@@ -2486,7 +2846,7 @@
         <v>99</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>97</v>
@@ -2503,18 +2863,17 @@
       <c r="H7" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="I7" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="12" t="s">
         <v>63</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C8" s="5"/>
+      <c r="C8" s="5" t="s">
+        <v>98</v>
+      </c>
       <c r="D8" s="5" t="s">
         <v>98</v>
       </c>
@@ -2530,11 +2889,8 @@
       <c r="H8" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="I8" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="12" t="s">
         <v>64</v>
       </c>
@@ -2542,13 +2898,13 @@
         <v>99</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>97</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>101</v>
@@ -2559,11 +2915,8 @@
       <c r="H9" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="I9" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="38.700000000000003" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="10" spans="1:9" ht="38.700000000000003" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="12" t="s">
         <v>65</v>
       </c>
@@ -2571,31 +2924,28 @@
         <v>95</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="D10" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>97</v>
-      </c>
       <c r="G10" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="I10" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="J10" s="6" t="s">
+      <c r="I10" s="6" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="219.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="12" t="s">
         <v>66</v>
       </c>
@@ -2603,63 +2953,63 @@
         <v>99</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D11" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>103</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>96</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>103</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="J11" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="I11" s="6" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="12" t="s">
         <v>67</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>99</v>
       </c>
+      <c r="C12" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="D12" s="5" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>101</v>
       </c>
       <c r="F12" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>101</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>97</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="I12" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="12" t="s">
         <v>68</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>98</v>
       </c>
+      <c r="C13" s="5" t="s">
+        <v>98</v>
+      </c>
       <c r="D13" s="5" t="s">
         <v>98</v>
       </c>
@@ -2675,22 +3025,22 @@
       <c r="H13" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="I13" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="12" t="s">
         <v>69</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>111</v>
       </c>
+      <c r="C14" s="5" t="s">
+        <v>96</v>
+      </c>
       <c r="D14" s="5" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>97</v>
@@ -2701,11 +3051,8 @@
       <c r="H14" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="I14" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="12" t="s">
         <v>70</v>
       </c>
@@ -2713,7 +3060,7 @@
         <v>111</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>101</v>
@@ -2725,16 +3072,13 @@
         <v>101</v>
       </c>
       <c r="G15" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="H15" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="H15" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="12" t="s">
         <v>71</v>
       </c>
@@ -2742,7 +3086,7 @@
         <v>113</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>97</v>
@@ -2759,19 +3103,19 @@
       <c r="H16" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="I16" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="12" t="s">
         <v>72</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>99</v>
       </c>
+      <c r="C17" s="5" t="s">
+        <v>96</v>
+      </c>
       <c r="D17" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>97</v>
@@ -2780,23 +3124,22 @@
         <v>97</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="12" t="s">
         <v>73</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C18" s="5"/>
+      <c r="C18" s="5" t="s">
+        <v>98</v>
+      </c>
       <c r="D18" s="5" t="s">
         <v>98</v>
       </c>
@@ -2812,11 +3155,8 @@
       <c r="H18" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="I18" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="12" t="s">
         <v>74</v>
       </c>
@@ -2824,7 +3164,7 @@
         <v>99</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>97</v>
@@ -2833,19 +3173,16 @@
         <v>97</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>96</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="25.8" x14ac:dyDescent="0.55000000000000004">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="12" t="s">
         <v>75</v>
       </c>
@@ -2853,7 +3190,7 @@
         <v>116</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>101</v>
@@ -2870,18 +3207,17 @@
       <c r="H20" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="I20" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="12" t="s">
         <v>76</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C21" s="5"/>
+      <c r="C21" s="5" t="s">
+        <v>98</v>
+      </c>
       <c r="D21" s="5" t="s">
         <v>98</v>
       </c>
@@ -2897,17 +3233,17 @@
       <c r="H21" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="I21" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="12" t="s">
         <v>77</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>98</v>
       </c>
+      <c r="C22" s="5" t="s">
+        <v>98</v>
+      </c>
       <c r="D22" s="5" t="s">
         <v>98</v>
       </c>
@@ -2923,17 +3259,17 @@
       <c r="H22" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="I22" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="12" t="s">
         <v>78</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>98</v>
       </c>
+      <c r="C23" s="5" t="s">
+        <v>98</v>
+      </c>
       <c r="D23" s="5" t="s">
         <v>98</v>
       </c>
@@ -2949,18 +3285,17 @@
       <c r="H23" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="I23" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="12" t="s">
         <v>79</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C24" s="5"/>
+      <c r="C24" s="5" t="s">
+        <v>98</v>
+      </c>
       <c r="D24" s="5" t="s">
         <v>98</v>
       </c>
@@ -2976,33 +3311,30 @@
       <c r="H24" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="I24" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="12" t="s">
         <v>80</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>118</v>
       </c>
+      <c r="C25" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="D25" s="5" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="E25" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F25" s="5" t="s">
         <v>101</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>97</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>101</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="I25" s="5" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3013,19 +3345,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26BDC261-6B45-4E97-AC79-120896DD6D8A}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="10.89453125" style="13" customWidth="1"/>
     <col min="2" max="3" width="50.578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="40.578125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="57.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" ht="57.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="9" t="s">
         <v>81</v>
       </c>
@@ -3035,8 +3368,11 @@
       <c r="C1" s="16" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="25.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="D1" s="15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="25.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="12" t="s">
         <v>57</v>
       </c>
@@ -3047,15 +3383,18 @@
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="25.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" ht="25.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="12" t="s">
         <v>58</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="25.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="D3" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="25.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="12" t="s">
         <v>59</v>
       </c>
@@ -3065,8 +3404,11 @@
       <c r="C4" s="17" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="25.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="D4" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="25.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="12" t="s">
         <v>60</v>
       </c>
@@ -3076,24 +3418,33 @@
       <c r="C5" s="17" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D5" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="12" t="s">
         <v>61</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="51.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D6" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="51.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="12" t="s">
         <v>62</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="77.400000000000006" x14ac:dyDescent="0.55000000000000004">
+      <c r="D7" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="77.400000000000006" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="12" t="s">
         <v>63</v>
       </c>
@@ -3103,8 +3454,9 @@
       <c r="C8" s="5" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="25.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:4" ht="25.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="12" t="s">
         <v>64</v>
       </c>
@@ -3112,29 +3464,38 @@
       <c r="C9" s="5" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="51.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D9" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="51.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="12" t="s">
         <v>65</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D10" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="219.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="12" t="s">
         <v>66</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D11" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="12" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="12" t="s">
         <v>68</v>
       </c>
@@ -3145,20 +3506,23 @@
         <v>140</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="12" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="12" t="s">
         <v>70</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D15" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="12" t="s">
         <v>71</v>
       </c>
@@ -3168,13 +3532,16 @@
       <c r="C16" s="5" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D16" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="12" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="38.700000000000003" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:4" ht="38.700000000000003" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="12" t="s">
         <v>73</v>
       </c>
@@ -3184,8 +3551,9 @@
       <c r="C18" s="5" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D18" s="5"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="12" t="s">
         <v>74</v>
       </c>
@@ -3195,8 +3563,11 @@
       <c r="C19" s="5" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="25.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="D19" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="25.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="12" t="s">
         <v>75</v>
       </c>
@@ -3206,8 +3577,11 @@
       <c r="C20" s="5" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="180.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D20" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="180.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="12" t="s">
         <v>76</v>
       </c>
@@ -3217,8 +3591,9 @@
       <c r="C21" s="5" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="25.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="D21" s="5"/>
+    </row>
+    <row r="22" spans="1:4" ht="25.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="12" t="s">
         <v>77</v>
       </c>
@@ -3226,7 +3601,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="25.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:4" ht="25.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="12" t="s">
         <v>78</v>
       </c>
@@ -3237,15 +3612,16 @@
         <v>148</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="12" t="s">
         <v>79</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D24" s="5"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="12" t="s">
         <v>80</v>
       </c>

</xml_diff>

<commit_message>
Updates in the survey data
</commit_message>
<xml_diff>
--- a/survey_data.xlsx
+++ b/survey_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conso\OneDrive\Documents\GitHub\robot-barriers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C7FC29-D240-435C-AFA7-475E373E2A4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FDB187-1822-4655-9455-6105998D3EA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,6 @@
     <sheet name="Proctor Report" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="201">
   <si>
     <t>How many years of experience do you have in computer programming?</t>
   </si>
@@ -618,9 +617,6 @@
     <t>The information and resources are not always accessible, The information and resources are not concise and clear</t>
   </si>
   <si>
-    <t>it seemed very accessible. Unfortunately, I believe I was experienced enough with programming fundamentals to not need the documentation.</t>
-  </si>
-  <si>
     <t>I believe the paper documentation provided more than enough information on what to do. Everything else was common sense.</t>
   </si>
   <si>
@@ -637,6 +633,24 @@
   </si>
   <si>
     <t>The proctor forgot to close the experiment on the desktop application. He manually recorded the participant's time on his phone. The participant took 42 minutes to complete the experiment.</t>
+  </si>
+  <si>
+    <t>p04231833</t>
+  </si>
+  <si>
+    <t>p04241504</t>
+  </si>
+  <si>
+    <t>Videos (e.g., YouTube, Udemy), Lecture Materials (e.g., In-Class Slides, Lecture Notes)</t>
+  </si>
+  <si>
+    <t>The coffee cans kept on deforming, which did not allow them to roll down sometimes. Everything else went fine</t>
+  </si>
+  <si>
+    <t>I think block based programming can be easy for people to learn because a lot of the technical theory and stuff is abstracted away. It helps people learn programming at a very basic level which is useful.</t>
+  </si>
+  <si>
+    <t>It seemed very accessible. Unfortunately, I believe I was experienced enough with programming fundamentals to not need the documentation.</t>
   </si>
 </sst>
 </file>
@@ -1133,7 +1147,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="A28" sqref="A28:A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1167,7 +1181,7 @@
       </c>
       <c r="I1" s="22">
         <f>COUNTA(A2:A50)</f>
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -1278,7 +1292,7 @@
       </c>
       <c r="J5" s="25">
         <f>I5/$I$1</f>
-        <v>3.8461538461538464E-2</v>
+        <v>3.5714285714285712E-2</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1309,7 +1323,7 @@
       </c>
       <c r="J6" s="25">
         <f>I6/$I$1</f>
-        <v>0.46153846153846156</v>
+        <v>0.42857142857142855</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1336,11 +1350,11 @@
       </c>
       <c r="I7">
         <f>COUNTIF($B$2:$B$50, H7)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J7" s="25">
         <f>I7/$I$1</f>
-        <v>0.38461538461538464</v>
+        <v>0.42857142857142855</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1371,7 +1385,7 @@
       </c>
       <c r="J8" s="25">
         <f>I8/$I$1</f>
-        <v>0.11538461538461539</v>
+        <v>0.10714285714285714</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1451,7 +1465,7 @@
       </c>
       <c r="J11" s="25">
         <f>I11/$I$1</f>
-        <v>0.53846153846153844</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1478,11 +1492,11 @@
       </c>
       <c r="I12">
         <f>COUNTIF($C$2:$C$50, H12)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J12" s="25">
         <f>I12/$I$1</f>
-        <v>0.26923076923076922</v>
+        <v>0.32142857142857145</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1513,7 +1527,7 @@
       </c>
       <c r="J13" s="25">
         <f>I13/$I$1</f>
-        <v>0.15384615384615385</v>
+        <v>0.14285714285714285</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1575,7 +1589,7 @@
       </c>
       <c r="J15" s="25">
         <f>I15/$I$1</f>
-        <v>3.8461538461538464E-2</v>
+        <v>3.5714285714285712E-2</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1651,11 +1665,11 @@
       </c>
       <c r="I18">
         <f>COUNTIF($D$2:$D$50,H18)</f>
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J18" s="25">
         <f>I18/$I$1</f>
-        <v>0.84615384615384615</v>
+        <v>0.8571428571428571</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1686,7 +1700,7 @@
       </c>
       <c r="J19" s="25">
         <f>I19/$I$1</f>
-        <v>0.15384615384615385</v>
+        <v>0.14285714285714285</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1855,11 +1869,11 @@
       </c>
       <c r="I25">
         <f>COUNTIF($E$2:$E$50,H25)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J25" s="25">
         <f>I25/$I$1</f>
-        <v>0.57692307692307687</v>
+        <v>0.5714285714285714</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1886,11 +1900,11 @@
       </c>
       <c r="I26">
         <f>COUNTIF($E$2:$E$50,H26)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J26" s="25">
         <f>I26/$I$1</f>
-        <v>0.34615384615384615</v>
+        <v>0.35714285714285715</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1921,10 +1935,28 @@
       </c>
       <c r="J27" s="25">
         <f>I27/$I$1</f>
-        <v>7.6923076923076927E-2</v>
+        <v>7.1428571428571425E-2</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="H28" s="13" t="s">
         <v>178</v>
       </c>
@@ -1938,6 +1970,24 @@
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="H29" s="13" t="s">
         <v>179</v>
       </c>
@@ -1980,11 +2030,11 @@
       </c>
       <c r="I33">
         <f>COUNTIF($F$2:$F$50, H33)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J33" s="25">
         <f>I33/$I$1</f>
-        <v>3.8461538461538464E-2</v>
+        <v>0.10714285714285714</v>
       </c>
     </row>
     <row r="34" spans="8:10" x14ac:dyDescent="0.55000000000000004">
@@ -1997,7 +2047,7 @@
       </c>
       <c r="J34" s="25">
         <f>I34/$I$1</f>
-        <v>0.26923076923076922</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="35" spans="8:10" x14ac:dyDescent="0.55000000000000004">
@@ -2010,7 +2060,7 @@
       </c>
       <c r="J35" s="25">
         <f>I35/$I$1</f>
-        <v>0.65384615384615385</v>
+        <v>0.6071428571428571</v>
       </c>
     </row>
     <row r="36" spans="8:10" x14ac:dyDescent="0.55000000000000004">
@@ -2022,7 +2072,7 @@
       </c>
       <c r="J36" s="25">
         <f>I36/$I$1</f>
-        <v>3.8461538461538464E-2</v>
+        <v>3.5714285714285712E-2</v>
       </c>
     </row>
   </sheetData>
@@ -2035,10 +2085,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2073,7 +2123,7 @@
       </c>
       <c r="L1" s="22">
         <f>COUNTA(A2:A50)</f>
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="38.700000000000003" x14ac:dyDescent="0.55000000000000004">
@@ -2139,11 +2189,11 @@
       </c>
       <c r="H4" s="13">
         <f>COUNTIFS(B2:B50, "*Videos (e.g., YouTube, Udemy)*")</f>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I4" s="24">
         <f>H4/$L$1</f>
-        <v>0.92307692307692313</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>20</v>
@@ -2154,7 +2204,7 @@
       </c>
       <c r="M4" s="24">
         <f t="shared" ref="M4:M9" si="0">L4/$L$1</f>
-        <v>0.65384615384615385</v>
+        <v>0.6071428571428571</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="51.6" x14ac:dyDescent="0.55000000000000004">
@@ -2178,11 +2228,11 @@
       </c>
       <c r="H5" s="13">
         <f>COUNTIFS(B2:B50, "*Textbooks*")</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I5" s="24">
         <f t="shared" ref="I5:I10" si="1">H5/$L$1</f>
-        <v>0.34615384615384615</v>
+        <v>0.35714285714285715</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>168</v>
@@ -2193,7 +2243,7 @@
       </c>
       <c r="M5" s="24">
         <f t="shared" si="0"/>
-        <v>0.23076923076923078</v>
+        <v>0.21428571428571427</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="38.700000000000003" x14ac:dyDescent="0.55000000000000004">
@@ -2217,18 +2267,18 @@
       </c>
       <c r="I6" s="24">
         <f t="shared" si="1"/>
-        <v>3.8461538461538464E-2</v>
+        <v>3.5714285714285712E-2</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>44</v>
       </c>
       <c r="L6" s="13">
         <f>COUNTIFS(C2:C50, "*The information and resources are not in a form that is readily useable*")</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M6" s="24">
         <f t="shared" si="0"/>
-        <v>0.34615384615384615</v>
+        <v>0.35714285714285715</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="38.700000000000003" x14ac:dyDescent="0.55000000000000004">
@@ -2248,22 +2298,22 @@
       </c>
       <c r="H7" s="13">
         <f>COUNTIFS(B2:B50, "*Online Communities (e.g., Reddit, Stack Overflow)*")</f>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I7" s="24">
         <f t="shared" si="1"/>
-        <v>0.76923076923076927</v>
+        <v>0.7857142857142857</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>42</v>
       </c>
       <c r="L7" s="13">
         <f>COUNTIFS(C2:C50, "*The information and resources are not concise and clear*")</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M7" s="24">
         <f t="shared" si="0"/>
-        <v>0.53846153846153844</v>
+        <v>0.5357142857142857</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="64.5" x14ac:dyDescent="0.55000000000000004">
@@ -2283,22 +2333,22 @@
       </c>
       <c r="H8" s="13">
         <f>COUNTIFS(B2:B50, "*Lecture Materials (e.g., In-Class Slides, Lecture Notes)*")</f>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I8" s="24">
         <f t="shared" si="1"/>
-        <v>0.65384615384615385</v>
+        <v>0.6785714285714286</v>
       </c>
       <c r="K8" s="4" t="s">
         <v>51</v>
       </c>
       <c r="L8" s="13">
         <f>COUNTIFS(C2:C50, "*The information and resources are not organized into logical and understandable components*")</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M8" s="24">
         <f t="shared" si="0"/>
-        <v>0.61538461538461542</v>
+        <v>0.6071428571428571</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="51.6" x14ac:dyDescent="0.55000000000000004">
@@ -2322,11 +2372,11 @@
       </c>
       <c r="H9" s="13">
         <f>COUNTIFS(B2:B50, "*Chatbots (e.g., ChatGPT)*")</f>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I9" s="24">
         <f t="shared" si="1"/>
-        <v>0.76923076923076927</v>
+        <v>0.7857142857142857</v>
       </c>
       <c r="K9" s="4" t="s">
         <v>169</v>
@@ -2337,7 +2387,7 @@
       </c>
       <c r="M9" s="24">
         <f t="shared" si="0"/>
-        <v>0.26923076923076922</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="51.6" x14ac:dyDescent="0.55000000000000004">
@@ -2357,11 +2407,11 @@
       </c>
       <c r="H10" s="13">
         <f>COUNTIFS(B2:B50, "*Technical Documentation*")</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I10" s="24">
         <f t="shared" si="1"/>
-        <v>0.38461538461538464</v>
+        <v>0.42857142857142855</v>
       </c>
       <c r="K10" s="4"/>
     </row>
@@ -2427,22 +2477,22 @@
       </c>
       <c r="H13" s="13">
         <f>COUNTIFS(D2:D50, "*Videos (e.g., YouTube, Udemy)*")</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I13" s="24">
         <f>H13/$L$1</f>
-        <v>0.30769230769230771</v>
+        <v>0.32142857142857145</v>
       </c>
       <c r="K13" s="4" t="s">
         <v>20</v>
       </c>
       <c r="L13" s="13">
         <f>COUNTIFS(E2:E50, "*The materials do not provide the sufficient or required information*")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M13" s="24">
         <f t="shared" ref="M13:M18" si="2">L13/$L$1</f>
-        <v>0.11538461538461539</v>
+        <v>0.14285714285714285</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="38.700000000000003" x14ac:dyDescent="0.55000000000000004">
@@ -2466,18 +2516,18 @@
       </c>
       <c r="I14" s="24">
         <f t="shared" ref="I14:I19" si="3">H14/$L$1</f>
-        <v>3.8461538461538464E-2</v>
+        <v>3.5714285714285712E-2</v>
       </c>
       <c r="K14" s="4" t="s">
         <v>168</v>
       </c>
       <c r="L14" s="13">
         <f>COUNTIFS(E2:E50, "*The information and resources are not always accessible*")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M14" s="24">
         <f t="shared" si="2"/>
-        <v>0.15384615384615385</v>
+        <v>0.17857142857142858</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2512,11 +2562,11 @@
       </c>
       <c r="L15" s="13">
         <f>COUNTIFS(E3:E51, "*The information and resources are not always accessible*")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M15" s="24">
         <f t="shared" si="2"/>
-        <v>0.15384615384615385</v>
+        <v>0.17857142857142858</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2540,18 +2590,18 @@
       </c>
       <c r="I16" s="24">
         <f t="shared" si="3"/>
-        <v>0.19230769230769232</v>
+        <v>0.17857142857142858</v>
       </c>
       <c r="K16" s="4" t="s">
         <v>42</v>
       </c>
       <c r="L16" s="13">
         <f>COUNTIFS(E4:E52, "*The information and resources are not always accessible*")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M16" s="24">
         <f t="shared" si="2"/>
-        <v>0.15384615384615385</v>
+        <v>0.17857142857142858</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2571,22 +2621,22 @@
       </c>
       <c r="H17" s="13">
         <f>COUNTIFS(D2:D50, "*Lecture Materials (e.g., In-Class Slides, Lecture Notes)*")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I17" s="24">
         <f t="shared" si="3"/>
-        <v>0.11538461538461539</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="K17" s="4" t="s">
         <v>51</v>
       </c>
       <c r="L17" s="13">
         <f>COUNTIFS(E5:E53, "*The information and resources are not always accessible*")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M17" s="24">
         <f t="shared" si="2"/>
-        <v>0.15384615384615385</v>
+        <v>0.17857142857142858</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="64.5" x14ac:dyDescent="0.55000000000000004">
@@ -2610,18 +2660,18 @@
       </c>
       <c r="I18" s="24">
         <f t="shared" si="3"/>
-        <v>0.26923076923076922</v>
+        <v>0.25</v>
       </c>
       <c r="K18" s="4" t="s">
         <v>169</v>
       </c>
       <c r="L18" s="13">
         <f>COUNTIFS(E6:E54, "*The information and resources are not always accessible*")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M18" s="24">
         <f t="shared" si="2"/>
-        <v>0.11538461538461539</v>
+        <v>0.14285714285714285</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="38.700000000000003" x14ac:dyDescent="0.55000000000000004">
@@ -2649,7 +2699,7 @@
       </c>
       <c r="I19" s="24">
         <f t="shared" si="3"/>
-        <v>0.19230769230769232</v>
+        <v>0.17857142857142858</v>
       </c>
       <c r="K19" s="4"/>
     </row>
@@ -2769,6 +2819,34 @@
       <c r="E27" s="5" t="s">
         <v>188</v>
       </c>
+    </row>
+    <row r="28" spans="1:13" ht="51.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="38.700000000000003" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
     </row>
   </sheetData>
   <dataConsolidate function="countNums">
@@ -2785,10 +2863,10 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3486,7 +3564,7 @@
         <v>98</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J26" s="12"/>
       <c r="K26" s="12"/>
@@ -3519,6 +3597,58 @@
       <c r="I27" s="5"/>
       <c r="J27" s="12"/>
       <c r="K27" s="12"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>98</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3530,10 +3660,10 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26:D27"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A29" sqref="A28:A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3816,13 +3946,13 @@
         <v>183</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -3830,12 +3960,29 @@
         <v>184</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D27" s="5"/>
+    </row>
+    <row r="28" spans="1:4" ht="38.700000000000003" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="25.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C29" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3847,10 +3994,10 @@
   <sheetPr>
     <tabColor theme="2" tint="-9.9978637043366805E-2"/>
   </sheetPr>
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4237,7 +4384,7 @@
         <v>155</v>
       </c>
       <c r="E26" s="27" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -4254,6 +4401,36 @@
         <v>155</v>
       </c>
       <c r="E27" s="5"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="26">
+        <v>45405.643518518518</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="E28" s="5"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="26">
+        <v>45406.493055555555</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="E29" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updates on the survey data
</commit_message>
<xml_diff>
--- a/survey_data.xlsx
+++ b/survey_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conso\OneDrive\Documents\GitHub\robot-barriers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FDB187-1822-4655-9455-6105998D3EA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD940EDD-F5C8-407F-B16F-CEDE50DB2466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Former Programming Experience" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Proctor Report" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="229">
   <si>
     <t>How many years of experience do you have in computer programming?</t>
   </si>
@@ -651,6 +652,90 @@
   </si>
   <si>
     <t>It seemed very accessible. Unfortunately, I believe I was experienced enough with programming fundamentals to not need the documentation.</t>
+  </si>
+  <si>
+    <t>p05011504</t>
+  </si>
+  <si>
+    <t>p05011708</t>
+  </si>
+  <si>
+    <t>p05011842</t>
+  </si>
+  <si>
+    <t>p05021329</t>
+  </si>
+  <si>
+    <t>p05021458</t>
+  </si>
+  <si>
+    <t>p05021659</t>
+  </si>
+  <si>
+    <t>p05021829</t>
+  </si>
+  <si>
+    <t>Masters Student</t>
+  </si>
+  <si>
+    <t>Videos (e.g., YouTube, Udemy), Online Communities (e.g., Reddit, Stack Overflow), Lecture Materials (e.g., In-Class Slides, Lecture Notes), Chatbots (e.g., ChatGPT), Technical Documentation, GIT and Kaggle</t>
+  </si>
+  <si>
+    <t>The information and resources are not always accessible, The information and resources are not in a form that is readily useable, The information and resources are not concise and clear, The information and resources provided are not up to date</t>
+  </si>
+  <si>
+    <t>Videos (e.g., YouTube, Udemy), Textbooks, Audiobooks, Online Communities (e.g., Reddit, Stack Overflow), Lecture Materials (e.g., In-Class Slides, Lecture Notes), Chatbots (e.g., ChatGPT)</t>
+  </si>
+  <si>
+    <t>The materials do not provide the sufficient or required information, The information and resources are not concise and clear</t>
+  </si>
+  <si>
+    <t>Lecture Materials (e.g., In-Class Slides, Lecture Notes), Technical Documentation, practice coding problems</t>
+  </si>
+  <si>
+    <t>Online Communities (e.g., Reddit, Stack Overflow), Lecture Materials (e.g., In-Class Slides, Lecture Notes), Chatbots (e.g., ChatGPT), Technical Documentation</t>
+  </si>
+  <si>
+    <t>Textbooks, Lecture Materials (e.g., In-Class Slides, Lecture Notes)</t>
+  </si>
+  <si>
+    <t>The materials do not provide the sufficient or required information, The information and resources are not in a form that is readily useable</t>
+  </si>
+  <si>
+    <t>Watch, No categories were useful for me</t>
+  </si>
+  <si>
+    <t>Did not use any</t>
+  </si>
+  <si>
+    <t>It is pretty intuitive and simple to learn</t>
+  </si>
+  <si>
+    <t>I did not really use them. It was more helpful for me to</t>
+  </si>
+  <si>
+    <t>Learning material had a beautiful UI</t>
+  </si>
+  <si>
+    <t>Nothing</t>
+  </si>
+  <si>
+    <t>I had a very specific question &amp; it was hard for me to understand the solution based on the resources. For example: I wanted to understand how the prompts thing worked &amp; i couldn't quickly find a solution</t>
+  </si>
+  <si>
+    <t>Took like 10 extra minutes</t>
+  </si>
+  <si>
+    <t>The participant was unable to complete the experiment because the flex pendant displayed "initialization failed" and it froze on restart. It never was able to return to the menu in time.</t>
+  </si>
+  <si>
+    <t>Read</t>
+  </si>
+  <si>
+    <t>Most useful learning categories</t>
+  </si>
+  <si>
+    <t>Strongly Disagree</t>
   </si>
 </sst>
 </file>
@@ -705,7 +790,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -760,6 +845,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -774,7 +865,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -791,17 +882,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -836,24 +921,61 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="22" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1144,21 +1266,21 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:A29"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.89453125" style="11" customWidth="1"/>
-    <col min="2" max="6" width="40.578125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="40.26171875" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" style="9" customWidth="1"/>
+    <col min="2" max="6" width="40.5703125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="40.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="56.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:10" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
         <v>81</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -1176,16 +1298,16 @@
       <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="I1" s="22">
+      <c r="I1" s="19">
         <f>COUNTA(A2:A50)</f>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>57</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1194,33 +1316,33 @@
       <c r="C2" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="D2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>58</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="C3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="H3" s="3" t="s">
@@ -1233,8 +1355,8 @@
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>59</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -1246,88 +1368,88 @@
       <c r="D4" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I4">
+      <c r="H4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="22">
         <f>COUNTIF($B$2:$B$50, H4)</f>
         <v>0</v>
       </c>
-      <c r="J4" s="25">
+      <c r="J4" s="23">
         <f>I4/$I$1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="10" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>60</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="C5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="5" t="s">
         <v>3</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="22">
         <f>COUNTIF($B$2:$B$50, H5)</f>
         <v>1</v>
       </c>
-      <c r="J5" s="25">
+      <c r="J5" s="23">
         <f>I5/$I$1</f>
-        <v>3.5714285714285712E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="10" t="s">
+        <v>2.8571428571428571E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>61</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="2" t="s">
+      <c r="C6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>3</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="22">
         <f>COUNTIF($B$2:$B$50, H6)</f>
-        <v>12</v>
-      </c>
-      <c r="J6" s="25">
+        <v>14</v>
+      </c>
+      <c r="J6" s="23">
         <f>I6/$I$1</f>
-        <v>0.42857142857142855</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="10" t="s">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>62</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -1336,29 +1458,29 @@
       <c r="C7" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="2" t="s">
+      <c r="D7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>7</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="22">
         <f>COUNTIF($B$2:$B$50, H7)</f>
-        <v>12</v>
-      </c>
-      <c r="J7" s="25">
+        <v>16</v>
+      </c>
+      <c r="J7" s="23">
         <f>I7/$I$1</f>
-        <v>0.42857142857142855</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="10" t="s">
+        <v>0.45714285714285713</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>63</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -1367,29 +1489,29 @@
       <c r="C8" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="2" t="s">
+      <c r="D8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="22">
         <f>COUNTIF($B$2:$B$50, H8)</f>
-        <v>3</v>
-      </c>
-      <c r="J8" s="25">
+        <v>4</v>
+      </c>
+      <c r="J8" s="23">
         <f>I8/$I$1</f>
-        <v>0.10714285714285714</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="10" t="s">
+        <v>0.11428571428571428</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>64</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -1398,33 +1520,42 @@
       <c r="C9" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="2" t="s">
+      <c r="D9" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="10" t="s">
+      <c r="H9" s="22"/>
+      <c r="I9" s="22">
+        <f>SUM(I4:I8)</f>
+        <v>35</v>
+      </c>
+      <c r="J9" s="23">
+        <f>I9/$I$1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>65</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="2" t="s">
+      <c r="C10" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>3</v>
       </c>
       <c r="H10" s="3" t="s">
@@ -1437,39 +1568,39 @@
         <v>173</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="10" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
         <v>66</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" s="2" t="s">
+      <c r="C11" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I11">
+      <c r="H11" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I11" s="22">
         <f>COUNTIF($C$2:$C$50, H11)</f>
-        <v>14</v>
-      </c>
-      <c r="J11" s="25">
+        <v>19</v>
+      </c>
+      <c r="J11" s="23">
         <f>I11/$I$1</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="10" t="s">
+        <v>0.54285714285714282</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>67</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -1481,88 +1612,88 @@
       <c r="D12" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="5" t="s">
         <v>7</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="22">
         <f>COUNTIF($C$2:$C$50, H12)</f>
-        <v>9</v>
-      </c>
-      <c r="J12" s="25">
+        <v>10</v>
+      </c>
+      <c r="J12" s="23">
         <f>I12/$I$1</f>
-        <v>0.32142857142857145</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="10" t="s">
+        <v>0.2857142857142857</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>68</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13" s="2" t="s">
+      <c r="C13" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>3</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="22">
         <f>COUNTIF($C$2:$C$50, H13)</f>
-        <v>4</v>
-      </c>
-      <c r="J13" s="25">
+        <v>5</v>
+      </c>
+      <c r="J13" s="23">
         <f>I13/$I$1</f>
         <v>0.14285714285714285</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="10" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
         <v>69</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" s="2" t="s">
+      <c r="C14" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>3</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="22">
         <f>COUNTIF($C$2:$C$50, H14)</f>
         <v>0</v>
       </c>
-      <c r="J14" s="25">
+      <c r="J14" s="23">
         <f>I14/$I$1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="10" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>70</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -1574,61 +1705,70 @@
       <c r="D15" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H15" s="11" t="s">
+      <c r="H15" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="22">
         <f>COUNTIF($C$2:$C$50, H15)</f>
         <v>1</v>
       </c>
-      <c r="J15" s="25">
+      <c r="J15" s="23">
         <f>I15/$I$1</f>
-        <v>3.5714285714285712E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="10" t="s">
+        <v>2.8571428571428571E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
         <v>71</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F16" s="2" t="s">
+      <c r="C16" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="10" t="s">
+      <c r="H16" s="22"/>
+      <c r="I16" s="22">
+        <f>SUM(I11:I15)</f>
+        <v>35</v>
+      </c>
+      <c r="J16" s="23">
+        <f>I16/$I$1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
         <v>72</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F17" s="2" t="s">
+      <c r="C17" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>7</v>
       </c>
       <c r="H17" s="3" t="s">
@@ -1641,8 +1781,8 @@
         <v>173</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="10" t="s">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
         <v>73</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -1651,29 +1791,29 @@
       <c r="C18" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F18" s="2" t="s">
+      <c r="D18" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I18">
+      <c r="H18" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I18" s="22">
         <f>COUNTIF($D$2:$D$50,H18)</f>
-        <v>24</v>
-      </c>
-      <c r="J18" s="25">
+        <v>31</v>
+      </c>
+      <c r="J18" s="23">
         <f>I18/$I$1</f>
-        <v>0.8571428571428571</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="10" t="s">
+        <v>0.88571428571428568</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
         <v>74</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -1685,69 +1825,69 @@
       <c r="D19" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="5" t="s">
         <v>7</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="22">
         <f>COUNTIF($D$2:$D$50,H19)</f>
         <v>4</v>
       </c>
-      <c r="J19" s="25">
+      <c r="J19" s="23">
         <f>I19/$I$1</f>
-        <v>0.14285714285714285</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="10" t="s">
+        <v>0.11428571428571428</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
         <v>75</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F20" s="2" t="s">
+      <c r="C20" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" s="5" t="s">
         <v>3</v>
       </c>
       <c r="H20" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="22">
         <f>COUNTIF($D$2:$D$50,H20)</f>
         <v>0</v>
       </c>
-      <c r="J20" s="25">
+      <c r="J20" s="23">
         <f>I20/$I$1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="10" t="s">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
         <v>76</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E21" s="2" t="s">
+      <c r="C21" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F21" s="5" t="s">
@@ -1756,17 +1896,17 @@
       <c r="H21" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="22">
         <f>COUNTIF($D$2:$D$50,H21)</f>
         <v>0</v>
       </c>
-      <c r="J21" s="25">
+      <c r="J21" s="23">
         <f>I21/$I$1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="10" t="s">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
         <v>77</v>
       </c>
       <c r="B22" s="5" t="s">
@@ -1775,29 +1915,29 @@
       <c r="C22" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E22" s="2" t="s">
+      <c r="D22" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F22" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H22" s="11" t="s">
+      <c r="H22" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="22">
         <f>COUNTIF($D$2:$D$50,H22)</f>
         <v>0</v>
       </c>
-      <c r="J22" s="25">
+      <c r="J22" s="23">
         <f>I22/$I$1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="10" t="s">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
         <v>78</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -1806,33 +1946,42 @@
       <c r="C23" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E23" s="2" t="s">
+      <c r="D23" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F23" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="10" t="s">
+      <c r="H23" s="22"/>
+      <c r="I23" s="22">
+        <f>SUM(I18:I22)</f>
+        <v>35</v>
+      </c>
+      <c r="J23" s="23">
+        <f>I23/$I$1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
         <v>79</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F24" s="2" t="s">
+      <c r="C24" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" s="5" t="s">
         <v>3</v>
       </c>
       <c r="H24" s="3" t="s">
@@ -1845,70 +1994,70 @@
         <v>173</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="10" t="s">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
         <v>80</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F25" s="2" t="s">
+      <c r="C25" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F25" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H25" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="I25">
+      <c r="H25" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="I25" s="22">
         <f>COUNTIF($E$2:$E$50,H25)</f>
-        <v>16</v>
-      </c>
-      <c r="J25" s="25">
+        <v>21</v>
+      </c>
+      <c r="J25" s="23">
         <f>I25/$I$1</f>
-        <v>0.5714285714285714</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="12" t="s">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="D26" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="F26" s="12" t="s">
+      <c r="D26" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H26" s="13" t="s">
+      <c r="H26" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="22">
         <f>COUNTIF($E$2:$E$50,H26)</f>
-        <v>10</v>
-      </c>
-      <c r="J26" s="25">
+        <v>12</v>
+      </c>
+      <c r="J26" s="23">
         <f>I26/$I$1</f>
-        <v>0.35714285714285715</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="10" t="s">
+        <v>0.34285714285714286</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
         <v>184</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -1926,20 +2075,20 @@
       <c r="F27" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H27" s="13" t="s">
+      <c r="H27" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I27">
+      <c r="I27" s="22">
         <f>COUNTIF($E$2:$E$50,H27)</f>
         <v>2</v>
       </c>
-      <c r="J27" s="25">
+      <c r="J27" s="23">
         <f>I27/$I$1</f>
-        <v>7.1428571428571425E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="10" t="s">
+        <v>5.7142857142857141E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
         <v>195</v>
       </c>
       <c r="B28" s="5" t="s">
@@ -1957,20 +2106,20 @@
       <c r="F28" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H28" s="13" t="s">
+      <c r="H28" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="I28">
+      <c r="I28" s="22">
         <f>COUNTIF($E$2:$E$50,H28)</f>
         <v>0</v>
       </c>
-      <c r="J28" s="25">
+      <c r="J28" s="23">
         <f>I28/$I$1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="10" t="s">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
         <v>196</v>
       </c>
       <c r="B29" s="5" t="s">
@@ -1988,19 +2137,66 @@
       <c r="F29" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H29" s="13" t="s">
+      <c r="H29" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="I29">
+      <c r="I29" s="22">
         <f>COUNTIF($E$2:$E$50,H29)</f>
         <v>0</v>
       </c>
-      <c r="J29" s="25">
+      <c r="J29" s="23">
         <f>I29/$I$1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="H30" s="22"/>
+      <c r="I30" s="22">
+        <f>SUM(I25:I29)</f>
+        <v>35</v>
+      </c>
+      <c r="J30" s="23">
+        <f>I30/$I$1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="H31" s="3" t="s">
         <v>180</v>
       </c>
@@ -2011,68 +2207,169 @@
         <v>173</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="H32" s="13" t="s">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="22" t="s">
+        <v>203</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H32" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="I32">
+      <c r="I32" s="22">
         <f>COUNTIF($F$2:$F$50, H32)</f>
         <v>0</v>
       </c>
-      <c r="J32" s="25">
+      <c r="J32" s="23">
         <f>I32/$I$1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="8:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="H33" s="13" t="s">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H33" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="I33">
+      <c r="I33" s="22">
         <f>COUNTIF($F$2:$F$50, H33)</f>
         <v>3</v>
       </c>
-      <c r="J33" s="25">
+      <c r="J33" s="23">
         <f>I33/$I$1</f>
-        <v>0.10714285714285714</v>
-      </c>
-    </row>
-    <row r="34" spans="8:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="H34" s="13" t="s">
+        <v>8.5714285714285715E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F34" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I34">
+      <c r="H34" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I34" s="22">
         <f>COUNTIF($F$2:$F$50, H34)</f>
+        <v>9</v>
+      </c>
+      <c r="J34" s="23">
+        <f>I34/$I$1</f>
+        <v>0.25714285714285712</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="I35" s="22">
+        <f>COUNTIF($F$2:$F$50, H35)</f>
+        <v>21</v>
+      </c>
+      <c r="J35" s="23">
+        <f>I35/$I$1</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="22" t="s">
+        <v>207</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F36" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J34" s="25">
-        <f>I34/$I$1</f>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="35" spans="8:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="H35" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I35">
-        <f>COUNTIF($F$2:$F$50, H35)</f>
-        <v>17</v>
-      </c>
-      <c r="J35" s="25">
-        <f>I35/$I$1</f>
-        <v>0.6071428571428571</v>
-      </c>
-    </row>
-    <row r="36" spans="8:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="H36" s="13" t="s">
+      <c r="H36" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="I36">
+      <c r="I36" s="22">
+        <v>2</v>
+      </c>
+      <c r="J36" s="23">
+        <f>I36/$I$1</f>
+        <v>5.7142857142857141E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H37" s="22"/>
+      <c r="I37" s="22">
+        <f>SUM(I32:I36)</f>
+        <v>35</v>
+      </c>
+      <c r="J37" s="23">
+        <f>I37/$I$1</f>
         <v>1</v>
-      </c>
-      <c r="J36" s="25">
-        <f>I36/$I$1</f>
-        <v>3.5714285714285712E-2</v>
       </c>
     </row>
   </sheetData>
@@ -2085,49 +2382,52 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:M29"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:A29"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.89453125" style="13" customWidth="1"/>
-    <col min="2" max="5" width="50.578125" style="13" customWidth="1"/>
-    <col min="7" max="7" width="60.05078125" customWidth="1"/>
-    <col min="11" max="11" width="45.7890625" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" style="10" customWidth="1"/>
+    <col min="2" max="5" width="50.5703125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="22"/>
+    <col min="7" max="7" width="60" style="22" customWidth="1"/>
+    <col min="8" max="10" width="9.140625" style="22"/>
+    <col min="11" max="11" width="45.85546875" style="22" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="55.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:13" ht="55.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="K1" s="33" t="s">
         <v>171</v>
       </c>
-      <c r="L1" s="22">
+      <c r="L1" s="33">
         <f>COUNTA(A2:A50)</f>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="38.700000000000003" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
         <v>57</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -2136,40 +2436,35 @@
       <c r="C2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="12" t="s">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
         <v>58</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="34" t="s">
         <v>172</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="34" t="s">
         <v>173</v>
       </c>
-      <c r="K3" s="21" t="s">
+      <c r="K3" s="34" t="s">
         <v>167</v>
       </c>
-      <c r="L3" s="21" t="s">
+      <c r="L3" s="34" t="s">
         <v>172</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="M3" s="34" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="77.400000000000006" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="12" t="s">
+    <row r="4" spans="1:13" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
         <v>59</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -2184,31 +2479,31 @@
       <c r="E4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="10">
         <f>COUNTIFS(B2:B50, "*Videos (e.g., YouTube, Udemy)*")</f>
-        <v>26</v>
-      </c>
-      <c r="I4" s="24">
+        <v>30</v>
+      </c>
+      <c r="I4" s="35">
         <f>H4/$L$1</f>
-        <v>0.9285714285714286</v>
-      </c>
-      <c r="K4" s="4" t="s">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="K4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="13">
+      <c r="L4" s="10">
         <f>COUNTIFS(C2:C50, "*The materials do not provide the sufficient or required information*")</f>
-        <v>17</v>
-      </c>
-      <c r="M4" s="24">
+        <v>20</v>
+      </c>
+      <c r="M4" s="35">
         <f t="shared" ref="M4:M9" si="0">L4/$L$1</f>
-        <v>0.6071428571428571</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="51.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="12" t="s">
+        <v>0.5714285714285714</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
         <v>60</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -2223,31 +2518,31 @@
       <c r="E5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="10">
         <f>COUNTIFS(B2:B50, "*Textbooks*")</f>
-        <v>10</v>
-      </c>
-      <c r="I5" s="24">
+        <v>14</v>
+      </c>
+      <c r="I5" s="35">
         <f t="shared" ref="I5:I10" si="1">H5/$L$1</f>
-        <v>0.35714285714285715</v>
-      </c>
-      <c r="K5" s="4" t="s">
+        <v>0.4</v>
+      </c>
+      <c r="K5" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="L5" s="13">
+      <c r="L5" s="10">
         <f>COUNTIFS(C2:C50, "*The information and resources are not always accessible*")</f>
-        <v>6</v>
-      </c>
-      <c r="M5" s="24">
+        <v>8</v>
+      </c>
+      <c r="M5" s="35">
         <f t="shared" si="0"/>
-        <v>0.21428571428571427</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="38.700000000000003" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="12" t="s">
+        <v>0.22857142857142856</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
         <v>61</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -2256,33 +2551,31 @@
       <c r="C6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="10">
         <f>COUNTIFS(B2:B50, "*Audiobooks*")</f>
         <v>1</v>
       </c>
-      <c r="I6" s="24">
+      <c r="I6" s="35">
         <f t="shared" si="1"/>
-        <v>3.5714285714285712E-2</v>
-      </c>
-      <c r="K6" s="4" t="s">
+        <v>2.8571428571428571E-2</v>
+      </c>
+      <c r="K6" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="L6" s="13">
+      <c r="L6" s="10">
         <f>COUNTIFS(C2:C50, "*The information and resources are not in a form that is readily useable*")</f>
-        <v>10</v>
-      </c>
-      <c r="M6" s="24">
+        <v>14</v>
+      </c>
+      <c r="M6" s="35">
         <f t="shared" si="0"/>
-        <v>0.35714285714285715</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="38.700000000000003" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="12" t="s">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
         <v>62</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -2291,33 +2584,31 @@
       <c r="C7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="10">
         <f>COUNTIFS(B2:B50, "*Online Communities (e.g., Reddit, Stack Overflow)*")</f>
-        <v>22</v>
-      </c>
-      <c r="I7" s="24">
+        <v>27</v>
+      </c>
+      <c r="I7" s="35">
         <f t="shared" si="1"/>
-        <v>0.7857142857142857</v>
-      </c>
-      <c r="K7" s="4" t="s">
+        <v>0.77142857142857146</v>
+      </c>
+      <c r="K7" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="L7" s="13">
+      <c r="L7" s="10">
         <f>COUNTIFS(C2:C50, "*The information and resources are not concise and clear*")</f>
-        <v>15</v>
-      </c>
-      <c r="M7" s="24">
+        <v>20</v>
+      </c>
+      <c r="M7" s="35">
         <f t="shared" si="0"/>
-        <v>0.5357142857142857</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="64.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="12" t="s">
+        <v>0.5714285714285714</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
         <v>63</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -2326,33 +2617,31 @@
       <c r="C8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="10">
         <f>COUNTIFS(B2:B50, "*Lecture Materials (e.g., In-Class Slides, Lecture Notes)*")</f>
-        <v>19</v>
-      </c>
-      <c r="I8" s="24">
+        <v>26</v>
+      </c>
+      <c r="I8" s="35">
         <f t="shared" si="1"/>
-        <v>0.6785714285714286</v>
-      </c>
-      <c r="K8" s="4" t="s">
+        <v>0.74285714285714288</v>
+      </c>
+      <c r="K8" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="L8" s="13">
+      <c r="L8" s="10">
         <f>COUNTIFS(C2:C50, "*The information and resources are not organized into logical and understandable components*")</f>
-        <v>17</v>
-      </c>
-      <c r="M8" s="24">
+        <v>20</v>
+      </c>
+      <c r="M8" s="35">
         <f t="shared" si="0"/>
-        <v>0.6071428571428571</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="51.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="12" t="s">
+        <v>0.5714285714285714</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
         <v>64</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -2367,31 +2656,31 @@
       <c r="E9" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="13">
+      <c r="H9" s="10">
         <f>COUNTIFS(B2:B50, "*Chatbots (e.g., ChatGPT)*")</f>
-        <v>22</v>
-      </c>
-      <c r="I9" s="24">
+        <v>27</v>
+      </c>
+      <c r="I9" s="35">
         <f t="shared" si="1"/>
-        <v>0.7857142857142857</v>
-      </c>
-      <c r="K9" s="4" t="s">
+        <v>0.77142857142857146</v>
+      </c>
+      <c r="K9" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="L9" s="13">
+      <c r="L9" s="10">
         <f>COUNTIFS(C2:C50, "*The information and resources provided are not up to date*")</f>
-        <v>7</v>
-      </c>
-      <c r="M9" s="24">
+        <v>9</v>
+      </c>
+      <c r="M9" s="35">
         <f t="shared" si="0"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="51.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="12" t="s">
+        <v>0.25714285714285712</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
         <v>65</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -2400,23 +2689,21 @@
       <c r="C10" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="10">
         <f>COUNTIFS(B2:B50, "*Technical Documentation*")</f>
-        <v>12</v>
-      </c>
-      <c r="I10" s="24">
+        <v>15</v>
+      </c>
+      <c r="I10" s="35">
         <f t="shared" si="1"/>
         <v>0.42857142857142855</v>
       </c>
-      <c r="K10" s="4"/>
-    </row>
-    <row r="11" spans="1:13" ht="51.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="12" t="s">
+      <c r="K10" s="5"/>
+    </row>
+    <row r="11" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
         <v>66</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -2425,12 +2712,10 @@
       <c r="C11" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="K11" s="4"/>
-    </row>
-    <row r="12" spans="1:13" ht="25.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="12" t="s">
+      <c r="K11" s="5"/>
+    </row>
+    <row r="12" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
         <v>67</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -2439,29 +2724,27 @@
       <c r="C12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="G12" s="23" t="s">
+      <c r="G12" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="H12" s="23" t="s">
+      <c r="H12" s="24" t="s">
         <v>172</v>
       </c>
-      <c r="I12" s="23" t="s">
+      <c r="I12" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="K12" s="23" t="s">
+      <c r="K12" s="24" t="s">
         <v>170</v>
       </c>
-      <c r="L12" s="23" t="s">
+      <c r="L12" s="24" t="s">
         <v>172</v>
       </c>
-      <c r="M12" s="23" t="s">
+      <c r="M12" s="24" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="51.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="12" t="s">
+    <row r="13" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
         <v>68</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -2470,33 +2753,31 @@
       <c r="C13" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="H13" s="13">
+      <c r="H13" s="10">
         <f>COUNTIFS(D2:D50, "*Videos (e.g., YouTube, Udemy)*")</f>
-        <v>9</v>
-      </c>
-      <c r="I13" s="24">
+        <v>10</v>
+      </c>
+      <c r="I13" s="35">
         <f>H13/$L$1</f>
-        <v>0.32142857142857145</v>
-      </c>
-      <c r="K13" s="4" t="s">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="K13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="L13" s="13">
+      <c r="L13" s="10">
         <f>COUNTIFS(E2:E50, "*The materials do not provide the sufficient or required information*")</f>
-        <v>4</v>
-      </c>
-      <c r="M13" s="24">
+        <v>6</v>
+      </c>
+      <c r="M13" s="35">
         <f t="shared" ref="M13:M18" si="2">L13/$L$1</f>
-        <v>0.14285714285714285</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="38.700000000000003" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="12" t="s">
+        <v>0.17142857142857143</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
         <v>69</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -2505,33 +2786,31 @@
       <c r="C14" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="G14" s="13" t="s">
+      <c r="G14" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="13">
+      <c r="H14" s="10">
         <f>COUNTIFS(D2:D50, "*Textbooks*")</f>
-        <v>1</v>
-      </c>
-      <c r="I14" s="24">
+        <v>2</v>
+      </c>
+      <c r="I14" s="35">
         <f t="shared" ref="I14:I19" si="3">H14/$L$1</f>
-        <v>3.5714285714285712E-2</v>
-      </c>
-      <c r="K14" s="4" t="s">
+        <v>5.7142857142857141E-2</v>
+      </c>
+      <c r="K14" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="L14" s="13">
+      <c r="L14" s="10">
         <f>COUNTIFS(E2:E50, "*The information and resources are not always accessible*")</f>
-        <v>5</v>
-      </c>
-      <c r="M14" s="24">
+        <v>6</v>
+      </c>
+      <c r="M14" s="35">
         <f t="shared" si="2"/>
-        <v>0.17857142857142858</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="12" t="s">
+        <v>0.17142857142857143</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
         <v>70</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -2546,31 +2825,31 @@
       <c r="E15" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G15" s="13" t="s">
+      <c r="G15" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="H15" s="13">
+      <c r="H15" s="10">
         <f>COUNTIFS(D2:D50, "*Audiobooks*")</f>
-        <v>0</v>
-      </c>
-      <c r="I15" s="24">
+        <v>1</v>
+      </c>
+      <c r="I15" s="35">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="K15" s="4" t="s">
+        <v>2.8571428571428571E-2</v>
+      </c>
+      <c r="K15" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="L15" s="13">
+      <c r="L15" s="10">
         <f>COUNTIFS(E3:E51, "*The information and resources are not always accessible*")</f>
-        <v>5</v>
-      </c>
-      <c r="M15" s="24">
+        <v>6</v>
+      </c>
+      <c r="M15" s="35">
         <f t="shared" si="2"/>
-        <v>0.17857142857142858</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="12" t="s">
+        <v>0.17142857142857143</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
         <v>71</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -2579,33 +2858,31 @@
       <c r="C16" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="G16" s="13" t="s">
+      <c r="G16" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="H16" s="13">
+      <c r="H16" s="10">
         <f>COUNTIFS(D2:D50, "*Online Communities (e.g., Reddit, Stack Overflow)*")</f>
-        <v>5</v>
-      </c>
-      <c r="I16" s="24">
+        <v>6</v>
+      </c>
+      <c r="I16" s="35">
         <f t="shared" si="3"/>
-        <v>0.17857142857142858</v>
-      </c>
-      <c r="K16" s="4" t="s">
+        <v>0.17142857142857143</v>
+      </c>
+      <c r="K16" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="L16" s="13">
+      <c r="L16" s="10">
         <f>COUNTIFS(E4:E52, "*The information and resources are not always accessible*")</f>
-        <v>5</v>
-      </c>
-      <c r="M16" s="24">
+        <v>6</v>
+      </c>
+      <c r="M16" s="35">
         <f t="shared" si="2"/>
-        <v>0.17857142857142858</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="12" t="s">
+        <v>0.17142857142857143</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
         <v>72</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -2614,33 +2891,31 @@
       <c r="C17" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="G17" s="13" t="s">
+      <c r="G17" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="H17" s="13">
+      <c r="H17" s="10">
         <f>COUNTIFS(D2:D50, "*Lecture Materials (e.g., In-Class Slides, Lecture Notes)*")</f>
-        <v>4</v>
-      </c>
-      <c r="I17" s="24">
+        <v>5</v>
+      </c>
+      <c r="I17" s="35">
         <f t="shared" si="3"/>
         <v>0.14285714285714285</v>
       </c>
-      <c r="K17" s="4" t="s">
+      <c r="K17" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="L17" s="13">
+      <c r="L17" s="10">
         <f>COUNTIFS(E5:E53, "*The information and resources are not always accessible*")</f>
-        <v>5</v>
-      </c>
-      <c r="M17" s="24">
+        <v>6</v>
+      </c>
+      <c r="M17" s="35">
         <f t="shared" si="2"/>
-        <v>0.17857142857142858</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="64.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="12" t="s">
+        <v>0.17142857142857143</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="10" t="s">
         <v>73</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -2649,33 +2924,31 @@
       <c r="C18" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="G18" s="13" t="s">
+      <c r="G18" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="H18" s="13">
+      <c r="H18" s="10">
         <f>COUNTIFS(D2:D50, "*Chatbots (e.g., ChatGPT)*")</f>
-        <v>7</v>
-      </c>
-      <c r="I18" s="24">
+        <v>9</v>
+      </c>
+      <c r="I18" s="35">
         <f t="shared" si="3"/>
-        <v>0.25</v>
-      </c>
-      <c r="K18" s="4" t="s">
+        <v>0.25714285714285712</v>
+      </c>
+      <c r="K18" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="L18" s="13">
+      <c r="L18" s="10">
         <f>COUNTIFS(E6:E54, "*The information and resources are not always accessible*")</f>
-        <v>4</v>
-      </c>
-      <c r="M18" s="24">
+        <v>5</v>
+      </c>
+      <c r="M18" s="35">
         <f t="shared" si="2"/>
         <v>0.14285714285714285</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="38.700000000000003" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="12" t="s">
+    <row r="19" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A19" s="10" t="s">
         <v>74</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -2690,33 +2963,30 @@
       <c r="E19" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="H19" s="13">
+      <c r="H19" s="10">
         <f>COUNTIFS(D2:D50, "*Technical Documentation*")</f>
         <v>5</v>
       </c>
-      <c r="I19" s="24">
+      <c r="I19" s="35">
         <f t="shared" si="3"/>
-        <v>0.17857142857142858</v>
-      </c>
-      <c r="K19" s="4"/>
-    </row>
-    <row r="20" spans="1:13" ht="25.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="12" t="s">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="K19" s="5"/>
+    </row>
+    <row r="20" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A20" s="10" t="s">
         <v>75</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="4"/>
-      <c r="K20" s="8"/>
-    </row>
-    <row r="21" spans="1:13" ht="90.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="12" t="s">
+      <c r="K20" s="25"/>
+    </row>
+    <row r="21" spans="1:13" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A21" s="10" t="s">
         <v>76</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -2725,12 +2995,10 @@
       <c r="C21" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="K21" s="8"/>
-    </row>
-    <row r="22" spans="1:13" ht="38.700000000000003" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="12" t="s">
+      <c r="K21" s="25"/>
+    </row>
+    <row r="22" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A22" s="10" t="s">
         <v>77</v>
       </c>
       <c r="B22" s="5" t="s">
@@ -2739,12 +3007,10 @@
       <c r="C22" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="K22" s="8"/>
-    </row>
-    <row r="23" spans="1:13" ht="64.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="12" t="s">
+      <c r="K22" s="25"/>
+    </row>
+    <row r="23" spans="1:13" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="10" t="s">
         <v>78</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -2760,8 +3026,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="38.700000000000003" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="12" t="s">
+    <row r="24" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A24" s="10" t="s">
         <v>79</v>
       </c>
       <c r="B24" s="5" t="s">
@@ -2770,11 +3036,9 @@
       <c r="C24" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-    </row>
-    <row r="25" spans="1:13" ht="51.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="12" t="s">
+    </row>
+    <row r="25" spans="1:13" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="10" t="s">
         <v>80</v>
       </c>
       <c r="B25" s="5" t="s">
@@ -2783,11 +3047,9 @@
       <c r="C25" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-    </row>
-    <row r="26" spans="1:13" ht="64.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="12" t="s">
+    </row>
+    <row r="26" spans="1:13" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="10" t="s">
         <v>183</v>
       </c>
       <c r="B26" s="5" t="s">
@@ -2803,8 +3065,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="51.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="10" t="s">
+    <row r="27" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
         <v>184</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -2820,8 +3082,8 @@
         <v>188</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="51.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="10" t="s">
+    <row r="28" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A28" s="8" t="s">
         <v>195</v>
       </c>
       <c r="B28" s="5" t="s">
@@ -2837,16 +3099,112 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="38.700000000000003" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="10" t="s">
+    <row r="29" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A29" s="8" t="s">
         <v>196</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
+    </row>
+    <row r="30" spans="1:13" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="B30" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="C30" s="25" t="s">
+        <v>210</v>
+      </c>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+    </row>
+    <row r="31" spans="1:13" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A31" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="B31" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" s="25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A32" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="B32" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32" s="25" t="s">
+        <v>211</v>
+      </c>
+      <c r="E32" s="25" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A33" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="B33" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="25"/>
+      <c r="E33" s="25"/>
+    </row>
+    <row r="34" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A34" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="B34" s="25" t="s">
+        <v>213</v>
+      </c>
+      <c r="C34" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
+    </row>
+    <row r="35" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A35" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="B35" s="25" t="s">
+        <v>214</v>
+      </c>
+      <c r="C35" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35" s="25"/>
+      <c r="E35" s="25"/>
+    </row>
+    <row r="36" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A36" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="B36" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="C36" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="D36" s="25"/>
+      <c r="E36" s="25"/>
     </row>
   </sheetData>
   <dataConsolidate function="countNums">
@@ -2863,50 +3221,61 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:M56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:A29"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K50" sqref="K50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.89453125" style="13" customWidth="1"/>
-    <col min="2" max="8" width="40.578125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="40.578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" style="4" customWidth="1"/>
+    <col min="2" max="8" width="40.5703125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="40.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="7"/>
+    <col min="11" max="11" width="43.5703125" style="7" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="7" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="48.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:13" ht="48.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="13" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="12" t="s">
+      <c r="K1" s="33" t="s">
+        <v>171</v>
+      </c>
+      <c r="L1" s="33">
+        <f>COUNTA(A2:A50)</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>57</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -2930,9 +3299,10 @@
       <c r="H2" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="12" t="s">
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>58</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -2956,9 +3326,19 @@
       <c r="H3" s="5" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="12" t="s">
+      <c r="I3" s="4"/>
+      <c r="K3" s="37" t="s">
+        <v>227</v>
+      </c>
+      <c r="L3" s="37" t="s">
+        <v>172</v>
+      </c>
+      <c r="M3" s="37" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>59</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -2982,9 +3362,21 @@
       <c r="H4" s="5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="25.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="12" t="s">
+      <c r="I4" s="4"/>
+      <c r="K4" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="L4" s="5">
+        <f>COUNTIFS(B1:B49, "*Read*")</f>
+        <v>3</v>
+      </c>
+      <c r="M4" s="36">
+        <f>L4/$L$1</f>
+        <v>8.5714285714285715E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>60</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -3008,12 +3400,23 @@
       <c r="H5" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="5" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="12" t="s">
+      <c r="K5" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="L5" s="5">
+        <f>COUNTIFS(B1:B49, "*Watch*")</f>
+        <v>6</v>
+      </c>
+      <c r="M5" s="36">
+        <f>L5/$L$1</f>
+        <v>0.17142857142857143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>61</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -3037,9 +3440,21 @@
       <c r="H6" s="5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="12" t="s">
+      <c r="I6" s="4"/>
+      <c r="K6" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="L6" s="5">
+        <f>COUNTIFS(B1:B49, "*Chat*")</f>
+        <v>16</v>
+      </c>
+      <c r="M6" s="36">
+        <f>L6/$L$1</f>
+        <v>0.45714285714285713</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -3063,9 +3478,21 @@
       <c r="H7" s="5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="12" t="s">
+      <c r="I7" s="4"/>
+      <c r="K7" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="L7" s="5">
+        <f>COUNTIFS(B1:B49, "*No categories were useful for me*")</f>
+        <v>3</v>
+      </c>
+      <c r="M7" s="36">
+        <f>L7/$L$1</f>
+        <v>8.5714285714285715E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>63</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -3089,9 +3516,21 @@
       <c r="H8" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="12" t="s">
+      <c r="I8" s="4"/>
+      <c r="K8" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="L8" s="5">
+        <f>COUNTIFS(B1:B49, "*I did not use the desktop computer*")</f>
+        <v>15</v>
+      </c>
+      <c r="M8" s="36">
+        <f>L8/$L$1</f>
+        <v>0.42857142857142855</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>64</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -3115,9 +3554,13 @@
       <c r="H9" s="5" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="38.700000000000003" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="12" t="s">
+      <c r="I9" s="4"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="36"/>
+    </row>
+    <row r="10" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>65</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -3141,12 +3584,21 @@
       <c r="H10" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="I10" s="6" t="s">
+      <c r="I10" s="5" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="12" t="s">
+      <c r="K10" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="L10" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="M10" s="38" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>66</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -3170,12 +3622,23 @@
       <c r="H11" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="5" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="12" t="s">
+      <c r="K11" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="L11" s="7">
+        <f>COUNTIFS(C1:C49, "Strongly Agree")</f>
+        <v>3</v>
+      </c>
+      <c r="M11" s="36">
+        <f>L11/$L$1</f>
+        <v>8.5714285714285715E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>67</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -3199,9 +3662,21 @@
       <c r="H12" s="5" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="12" t="s">
+      <c r="I12" s="4"/>
+      <c r="K12" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="L12" s="7">
+        <f>COUNTIFS(C1:C49, "Agree")</f>
+        <v>10</v>
+      </c>
+      <c r="M12" s="36">
+        <f t="shared" ref="M12:M16" si="0">L12/$L$1</f>
+        <v>0.2857142857142857</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>68</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -3225,9 +3700,21 @@
       <c r="H13" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="12" t="s">
+      <c r="I13" s="4"/>
+      <c r="K13" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L13" s="7">
+        <f>COUNTIFS(C1:C49, "Neither Agree or Disagree")</f>
+        <v>5</v>
+      </c>
+      <c r="M13" s="36">
+        <f t="shared" si="0"/>
+        <v>0.14285714285714285</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>69</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -3251,9 +3738,21 @@
       <c r="H14" s="5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="12" t="s">
+      <c r="I14" s="4"/>
+      <c r="K14" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="L14" s="7">
+        <f>COUNTIFS(C1:C49, "Disagree")</f>
+        <v>2</v>
+      </c>
+      <c r="M14" s="36">
+        <f t="shared" si="0"/>
+        <v>5.7142857142857141E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>70</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -3277,9 +3776,21 @@
       <c r="H15" s="5" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="12" t="s">
+      <c r="I15" s="4"/>
+      <c r="K15" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="L15" s="7">
+        <f>COUNTIFS(C1:C49, "Strongly Disagree")</f>
+        <v>0</v>
+      </c>
+      <c r="M15" s="36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>71</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -3303,9 +3814,21 @@
       <c r="H16" s="5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="12" t="s">
+      <c r="I16" s="4"/>
+      <c r="K16" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="L16" s="7">
+        <f>COUNTIFS(C1:C49, "I did not use the desktop computer")</f>
+        <v>15</v>
+      </c>
+      <c r="M16" s="36">
+        <f t="shared" si="0"/>
+        <v>0.42857142857142855</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>72</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -3329,9 +3852,10 @@
       <c r="H17" s="5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="12" t="s">
+      <c r="I17" s="4"/>
+    </row>
+    <row r="18" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>73</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -3355,9 +3879,19 @@
       <c r="H18" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="12" t="s">
+      <c r="I18" s="4"/>
+      <c r="K18" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="L18" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="M18" s="38" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>74</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -3381,9 +3915,21 @@
       <c r="H19" s="5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="12" t="s">
+      <c r="I19" s="4"/>
+      <c r="K19" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="L19" s="7">
+        <f>COUNTIFS(D1:D49, "Strongly Agree")</f>
+        <v>9</v>
+      </c>
+      <c r="M19" s="36">
+        <f>L19/$L$1</f>
+        <v>0.25714285714285712</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>75</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -3407,9 +3953,21 @@
       <c r="H20" s="5" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="12" t="s">
+      <c r="I20" s="4"/>
+      <c r="K20" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="L20" s="7">
+        <f>COUNTIFS(D1:D49, "Agree")</f>
+        <v>8</v>
+      </c>
+      <c r="M20" s="36">
+        <f t="shared" ref="M20:M24" si="1">L20/$L$1</f>
+        <v>0.22857142857142856</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
         <v>76</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -3433,9 +3991,21 @@
       <c r="H21" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="12" t="s">
+      <c r="I21" s="4"/>
+      <c r="K21" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L21" s="7">
+        <f>COUNTIFS(D1:D49, "Neither Agree or Disagree")</f>
+        <v>2</v>
+      </c>
+      <c r="M21" s="36">
+        <f t="shared" si="1"/>
+        <v>5.7142857142857141E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>77</v>
       </c>
       <c r="B22" s="5" t="s">
@@ -3459,9 +4029,21 @@
       <c r="H22" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="12" t="s">
+      <c r="I22" s="4"/>
+      <c r="K22" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="L22" s="7">
+        <f>COUNTIFS(D1:D49, "Disagree")</f>
+        <v>1</v>
+      </c>
+      <c r="M22" s="36">
+        <f t="shared" si="1"/>
+        <v>2.8571428571428571E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>78</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -3485,9 +4067,21 @@
       <c r="H23" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="12" t="s">
+      <c r="I23" s="4"/>
+      <c r="K23" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="L23" s="7">
+        <f>COUNTIFS(D1:D49, "Strongly Disagree")</f>
+        <v>0</v>
+      </c>
+      <c r="M23" s="36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>79</v>
       </c>
       <c r="B24" s="5" t="s">
@@ -3511,9 +4105,21 @@
       <c r="H24" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="12" t="s">
+      <c r="I24" s="4"/>
+      <c r="K24" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="L24" s="7">
+        <f>COUNTIFS(D1:D49, "I did not use the desktop computer")</f>
+        <v>15</v>
+      </c>
+      <c r="M24" s="36">
+        <f t="shared" si="1"/>
+        <v>0.42857142857142855</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
         <v>80</v>
       </c>
       <c r="B25" s="5" t="s">
@@ -3537,9 +4143,10 @@
       <c r="H25" s="5" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" ht="38.700000000000003" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="12" t="s">
+      <c r="I25" s="4"/>
+    </row>
+    <row r="26" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
         <v>183</v>
       </c>
       <c r="B26" s="5" t="s">
@@ -3566,11 +4173,19 @@
       <c r="I26" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="10" t="s">
+      <c r="J26" s="5"/>
+      <c r="K26" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="L26" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="M26" s="38" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="27" t="s">
         <v>184</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -3595,11 +4210,21 @@
         <v>98</v>
       </c>
       <c r="I27" s="5"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="12" t="s">
+      <c r="J27" s="5"/>
+      <c r="K27" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="L27" s="7">
+        <f>COUNTIFS(E1:E49, "Strongly Agree")</f>
+        <v>6</v>
+      </c>
+      <c r="M27" s="36">
+        <f>L27/$L$1</f>
+        <v>0.17142857142857143</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
         <v>195</v>
       </c>
       <c r="B28" s="5" t="s">
@@ -3623,9 +4248,21 @@
       <c r="H28" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="12" t="s">
+      <c r="I28" s="4"/>
+      <c r="K28" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="L28" s="7">
+        <f>COUNTIFS(E1:E49, "Agree")</f>
+        <v>11</v>
+      </c>
+      <c r="M28" s="36">
+        <f t="shared" ref="M28:M32" si="2">L28/$L$1</f>
+        <v>0.31428571428571428</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
         <v>196</v>
       </c>
       <c r="B29" s="5" t="s">
@@ -3648,6 +4285,503 @@
       </c>
       <c r="H29" s="5" t="s">
         <v>98</v>
+      </c>
+      <c r="I29" s="4"/>
+      <c r="K29" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L29" s="7">
+        <f>COUNTIFS(E1:E49, "Neither Agree or Disagree")</f>
+        <v>2</v>
+      </c>
+      <c r="M29" s="36">
+        <f t="shared" si="2"/>
+        <v>5.7142857142857141E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="28" t="s">
+        <v>201</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="D30" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="E30" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="F30" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="G30" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="H30" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="I30" s="29"/>
+      <c r="K30" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="L30" s="7">
+        <f>COUNTIFS(E1:E49, "Disagree")</f>
+        <v>1</v>
+      </c>
+      <c r="M30" s="36">
+        <f t="shared" si="2"/>
+        <v>2.8571428571428571E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="28" t="s">
+        <v>202</v>
+      </c>
+      <c r="B31" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="C31" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="D31" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="E31" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="F31" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="G31" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="H31" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="I31" s="29"/>
+      <c r="K31" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="L31" s="7">
+        <f>COUNTIFS(E1:E49, "Strongly Disagree")</f>
+        <v>0</v>
+      </c>
+      <c r="M31" s="36">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="B32" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="D32" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="E32" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="F32" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="G32" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="H32" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="I32" s="29"/>
+      <c r="K32" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="L32" s="7">
+        <f>COUNTIFS(E1:E49, "I did not use the desktop computer")</f>
+        <v>15</v>
+      </c>
+      <c r="M32" s="36">
+        <f t="shared" si="2"/>
+        <v>0.42857142857142855</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="64.5" x14ac:dyDescent="0.25">
+      <c r="A33" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="B33" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="C33" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="D33" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="E33" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="F33" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="G33" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="H33" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="I33" s="28" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A34" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C34" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="D34" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="E34" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="F34" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="G34" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="H34" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="I34" s="29"/>
+      <c r="K34" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="L34" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="M34" s="38" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="28" t="s">
+        <v>206</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C35" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="D35" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="E35" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="F35" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="G35" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="H35" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="I35" s="29"/>
+      <c r="K35" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="L35" s="7">
+        <f>COUNTIFS(F1:F49, "Strongly Agree")</f>
+        <v>6</v>
+      </c>
+      <c r="M35" s="36">
+        <f>L35/$L$1</f>
+        <v>0.17142857142857143</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="28" t="s">
+        <v>207</v>
+      </c>
+      <c r="B36" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="D36" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="E36" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="F36" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="G36" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="H36" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="I36" s="29"/>
+      <c r="K36" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="L36" s="7">
+        <f>COUNTIFS(F1:F49, "Agree")</f>
+        <v>10</v>
+      </c>
+      <c r="M36" s="36">
+        <f t="shared" ref="M36:M54" si="3">L36/$L$1</f>
+        <v>0.2857142857142857</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K37" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L37" s="7">
+        <f>COUNTIFS(F1:F49, "Neither Agree or Disagree")</f>
+        <v>3</v>
+      </c>
+      <c r="M37" s="36">
+        <f t="shared" si="3"/>
+        <v>8.5714285714285715E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K38" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="L38" s="7">
+        <f>COUNTIFS(F1:F49, "Disagree")</f>
+        <v>1</v>
+      </c>
+      <c r="M38" s="36">
+        <f t="shared" si="3"/>
+        <v>2.8571428571428571E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K39" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="L39" s="7">
+        <f>COUNTIFS(F1:F49, "Strongly Disagree")</f>
+        <v>0</v>
+      </c>
+      <c r="M39" s="36">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K40" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="L40" s="7">
+        <f>COUNTIFS(F1:F49, "I did not use the desktop computer")</f>
+        <v>15</v>
+      </c>
+      <c r="M40" s="36">
+        <f t="shared" si="3"/>
+        <v>0.42857142857142855</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="K42" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="L42" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="M42" s="38" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K43" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="L43" s="7">
+        <f>COUNTIFS(G1:G49, "Strongly Agree")</f>
+        <v>5</v>
+      </c>
+      <c r="M43" s="36">
+        <f>L43/$L$1</f>
+        <v>0.14285714285714285</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K44" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="L44" s="7">
+        <f>COUNTIFS(G1:G49, "Agree")</f>
+        <v>9</v>
+      </c>
+      <c r="M44" s="36">
+        <f>L44/$L$1</f>
+        <v>0.25714285714285712</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K45" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L45" s="7">
+        <f>COUNTIFS(G1:G49, "Neither Agree or Disagree")</f>
+        <v>5</v>
+      </c>
+      <c r="M45" s="36">
+        <f>L45/$L$1</f>
+        <v>0.14285714285714285</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K46" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="L46" s="7">
+        <f>COUNTIFS(G1:G49, "Disagree")</f>
+        <v>1</v>
+      </c>
+      <c r="M46" s="36">
+        <f>L46/$L$1</f>
+        <v>2.8571428571428571E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K47" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="L47" s="7">
+        <f>COUNTIFS(G1:G49, "Strongly Disagree")</f>
+        <v>0</v>
+      </c>
+      <c r="M47" s="36">
+        <f>L47/$L$1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K48" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="L48" s="7">
+        <f>COUNTIFS(G1:G49, "I did not use the desktop computer")</f>
+        <v>15</v>
+      </c>
+      <c r="M48" s="36">
+        <f>L48/$L$1</f>
+        <v>0.42857142857142855</v>
+      </c>
+    </row>
+    <row r="50" spans="11:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="K50" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="L50" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="M50" s="38" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="51" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K51" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="L51" s="7">
+        <f>COUNTIFS(H1:H49, "Strongly Agree")</f>
+        <v>8</v>
+      </c>
+      <c r="M51" s="36">
+        <f>L51/$L$1</f>
+        <v>0.22857142857142856</v>
+      </c>
+    </row>
+    <row r="52" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K52" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="L52" s="7">
+        <f>COUNTIFS(H1:H49, "Agree")</f>
+        <v>10</v>
+      </c>
+      <c r="M52" s="36">
+        <f>L52/$L$1</f>
+        <v>0.2857142857142857</v>
+      </c>
+    </row>
+    <row r="53" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K53" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L53" s="7">
+        <f>COUNTIFS(H1:H49, "Neither Agree or Disagree")</f>
+        <v>2</v>
+      </c>
+      <c r="M53" s="36">
+        <f>L53/$L$1</f>
+        <v>5.7142857142857141E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K54" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="L54" s="7">
+        <f>COUNTIFS(H1:H49, "Disagree")</f>
+        <v>0</v>
+      </c>
+      <c r="M54" s="36">
+        <f>L54/$L$1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K55" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="L55" s="7">
+        <f>COUNTIFS(H1:H49, "Strongly Disagree")</f>
+        <v>0</v>
+      </c>
+      <c r="M55" s="36">
+        <f>L55/$L$1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K56" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="L56" s="7">
+        <f>COUNTIFS(H1:H49, "I did not use the desktop computer")</f>
+        <v>15</v>
+      </c>
+      <c r="M56" s="36">
+        <f>L56/$L$1</f>
+        <v>0.42857142857142855</v>
       </c>
     </row>
   </sheetData>
@@ -3660,85 +4794,85 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A29" sqref="A28:A29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.89453125" style="13" customWidth="1"/>
-    <col min="2" max="3" width="50.578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="40.578125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" style="11" customWidth="1"/>
+    <col min="2" max="3" width="50.5703125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="40.5703125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="57.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:4" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="13" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="25.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>57</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="15" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="25.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="15" t="s">
         <v>134</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="25.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="12" t="s">
+    <row r="4" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>59</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="15" t="s">
         <v>134</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="25.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="12" t="s">
+    <row r="5" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>60</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="15" t="s">
         <v>134</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="12" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>61</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -3748,8 +4882,8 @@
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="51.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="12" t="s">
+    <row r="7" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -3759,8 +4893,8 @@
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="77.400000000000006" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="12" t="s">
+    <row r="8" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>63</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -3771,8 +4905,8 @@
       </c>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:4" ht="25.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="12" t="s">
+    <row r="9" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>64</v>
       </c>
       <c r="B9" s="5"/>
@@ -3783,8 +4917,8 @@
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="51.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="12" t="s">
+    <row r="10" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>65</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -3794,8 +4928,8 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="219.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="12" t="s">
+    <row r="11" spans="1:4" ht="242.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>66</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -3805,13 +4939,13 @@
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="12" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="12" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>68</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -3821,13 +4955,13 @@
         <v>140</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="12" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="12" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>70</v>
       </c>
       <c r="C15" s="5" t="s">
@@ -3837,8 +4971,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="12" t="s">
+    <row r="16" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>71</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -3851,13 +4985,13 @@
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="12" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="38.700000000000003" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="12" t="s">
+    <row r="18" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>73</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -3868,8 +5002,8 @@
       </c>
       <c r="D18" s="5"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="12" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>74</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -3882,8 +5016,8 @@
         <v>115</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="25.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="12" t="s">
+    <row r="20" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>75</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -3896,8 +5030,8 @@
         <v>117</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="180.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="12" t="s">
+    <row r="21" spans="1:4" ht="204" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
         <v>76</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -3908,16 +5042,16 @@
       </c>
       <c r="D21" s="5"/>
     </row>
-    <row r="22" spans="1:4" ht="25.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="12" t="s">
+    <row r="22" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>77</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="25.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="12" t="s">
+    <row r="23" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>78</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -3927,8 +5061,8 @@
         <v>148</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="12" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>79</v>
       </c>
       <c r="C24" s="5" t="s">
@@ -3936,13 +5070,13 @@
       </c>
       <c r="D24" s="5"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="12" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="38.700000000000003" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="12" t="s">
+    <row r="26" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
         <v>183</v>
       </c>
       <c r="B26" s="5" t="s">
@@ -3955,8 +5089,8 @@
         <v>200</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="10" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
         <v>184</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -3967,22 +5101,72 @@
       </c>
       <c r="D27" s="5"/>
     </row>
-    <row r="28" spans="1:4" ht="38.700000000000003" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="12" t="s">
+    <row r="28" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
         <v>195</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="25.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="12" t="s">
+    <row r="29" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
         <v>196</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>198</v>
       </c>
       <c r="C29" s="5"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>221</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3994,36 +5178,36 @@
   <sheetPr>
     <tabColor theme="2" tint="-9.9978637043366805E-2"/>
   </sheetPr>
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="50.578125" style="4" customWidth="1"/>
+    <col min="1" max="5" width="50.5703125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="67.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:5" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="12" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="18">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="16">
         <v>45392.5118530787</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -4036,8 +5220,8 @@
         <v>155</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="18">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="16">
         <v>45392.646322256944</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -4050,8 +5234,8 @@
         <v>156</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="51.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="18">
+    <row r="4" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="16">
         <v>45392.712318275459</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -4063,12 +5247,12 @@
       <c r="D4" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="17" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="18">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="16">
         <v>45393.51467798611</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -4081,8 +5265,8 @@
         <v>155</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="18">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="16">
         <v>45393.603960092594</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -4095,8 +5279,8 @@
         <v>155</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="18">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="16">
         <v>45393.653702118056</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -4109,8 +5293,8 @@
         <v>156</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="18">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="16">
         <v>45393.718732986112</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -4123,8 +5307,8 @@
         <v>155</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="18">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="16">
         <v>45394.451897141204</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -4137,8 +5321,8 @@
         <v>155</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="219.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="18">
+    <row r="10" spans="1:5" ht="242.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="16">
         <v>45394.517322256943</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -4150,12 +5334,12 @@
       <c r="D10" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="15" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="18">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="16">
         <v>45394.592569606481</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -4168,8 +5352,8 @@
         <v>156</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="18">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="16">
         <v>45394.650823310185</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -4182,8 +5366,8 @@
         <v>155</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="18">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="16">
         <v>45394.711310451385</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -4196,8 +5380,8 @@
         <v>155</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="18">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="16">
         <v>45397.582289699072</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -4210,8 +5394,8 @@
         <v>155</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="18">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="16">
         <v>45397.663417025462</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -4224,8 +5408,8 @@
         <v>155</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="18">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="16">
         <v>45397.716173460649</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -4238,8 +5422,8 @@
         <v>155</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="18">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="16">
         <v>45398.458225312497</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -4252,8 +5436,8 @@
         <v>156</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="25.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="18">
+    <row r="18" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="16">
         <v>45398.637042881943</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -4265,12 +5449,12 @@
       <c r="D18" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="E18" s="19" t="s">
+      <c r="E18" s="17" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="18">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="16">
         <v>45399.515523819442</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -4283,8 +5467,8 @@
         <v>156</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="90.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="18">
+    <row r="20" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="16">
         <v>45399.66549944444</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -4296,12 +5480,12 @@
       <c r="D20" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="E20" s="17" t="s">
+      <c r="E20" s="15" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="18">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="16">
         <v>45400.500941493054</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -4314,8 +5498,8 @@
         <v>155</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="18">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="16">
         <v>45400.57352726852</v>
       </c>
       <c r="B22" s="5" t="s">
@@ -4328,8 +5512,8 @@
         <v>155</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="18">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="16">
         <v>45401.59849498843</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -4342,8 +5526,8 @@
         <v>155</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="18">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="16">
         <v>45401.648354687495</v>
       </c>
       <c r="B24" s="5" t="s">
@@ -4356,8 +5540,8 @@
         <v>155</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="18">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="16">
         <v>45401.729860995372</v>
       </c>
       <c r="B25" s="5" t="s">
@@ -4370,11 +5554,11 @@
         <v>155</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="39" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="26">
+    <row r="26" spans="1:5" ht="51" x14ac:dyDescent="0.25">
+      <c r="A26" s="20">
         <v>45404.704814814817</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="5" t="s">
         <v>183</v>
       </c>
       <c r="C26" s="5" t="s">
@@ -4383,15 +5567,15 @@
       <c r="D26" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="E26" s="27" t="s">
+      <c r="E26" s="30" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="26">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="20">
         <v>45405.582685185182</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="5" t="s">
         <v>184</v>
       </c>
       <c r="C27" s="5" t="s">
@@ -4402,11 +5586,11 @@
       </c>
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="26">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="20">
         <v>45405.643518518518</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="5" t="s">
         <v>195</v>
       </c>
       <c r="C28" s="5" t="s">
@@ -4417,11 +5601,11 @@
       </c>
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="26">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="20">
         <v>45406.493055555555</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="5" t="s">
         <v>196</v>
       </c>
       <c r="C29" s="5" t="s">
@@ -4431,6 +5615,110 @@
         <v>156</v>
       </c>
       <c r="E29" s="5"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="31">
+        <v>45413.488439733796</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="31">
+        <v>45413.604592905089</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E31" s="32" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="31">
+        <v>45413.649242476851</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="31">
+        <v>45414.441224490743</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="31">
+        <v>45414.504462430559</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="51" x14ac:dyDescent="0.25">
+      <c r="A35" s="31">
+        <v>45414.587939571764</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E35" s="32" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="31">
+        <v>45414.665006203708</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>156</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>